<commit_message>
notes week 10 complete
Signed-off-by: the-other-mariana <mariana.avalos.arce@gmail.com>
</commit_message>
<xml_diff>
--- a/week9/ValueIteration.xlsx
+++ b/week9/ValueIteration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\github-mariana\ECID2\rl\week9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3F28DC-A0A0-4673-90AC-F45956E2550A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D33348-1EE3-4E0B-B8FC-5A4BF9718EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{76B46E62-252C-4031-B4FC-38427F8B6B71}"/>
   </bookViews>
@@ -730,7 +730,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>